<commit_message>
Updating City, Community and Building TCs..
</commit_message>
<xml_diff>
--- a/TestData/RegressionTestData.xlsx
+++ b/TestData/RegressionTestData.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectRegistration" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="City" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Communities" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Building" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="165">
   <si>
     <t xml:space="preserve">CityProjectName</t>
   </si>
@@ -283,6 +284,258 @@
   </si>
   <si>
     <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_OperatingHours_Hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_OperatingHours_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_GrossArea_GrossArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Occupant_RegularOccupant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Occupant_DaysPerWeek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Occupant_NoOfVisitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_GrossArea_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Occupant_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Odays_Days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Odays_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Emissions_Values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS_Emissions_Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy_Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy_FuelSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energy_Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_FuelSource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water_Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Generated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Diverted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waste_Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Walk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Bike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_TeleCommute</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Motorcycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_RapidTransit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Carpool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_CarAlternate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_LightRail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_CarSolo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport_Occupant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CO2_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TVOC_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM2.5_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ozone_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CarbonMonoxide_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acetaldehyde_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benzene_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Styrene_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toluene_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nepthalene_Reading</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color rgb="FF3F7F5F"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">Dichlorobenzene</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">_Reading</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Formaldehyde_Reading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operating Hours Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Floor Area Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Occupant Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operational Days Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissions Remarks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kWh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generated onsite - wind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mgal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reclaimed onsite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Auto Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Auto Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Auto Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular Occupant</t>
   </si>
 </sst>
 </file>
@@ -292,7 +545,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -327,6 +580,19 @@
       <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF3F7F5F"/>
+      <name val="Consolas"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val=""/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -372,7 +638,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -386,6 +652,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -449,7 +719,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF3F7F5F"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -468,11 +738,11 @@
   </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="BA2 N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.06"/>
@@ -617,7 +887,7 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="BA2 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -629,7 +899,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="65" style="1" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.57"/>
   </cols>
@@ -903,7 +1173,7 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="BA2 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -915,7 +1185,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="65" style="1" width="11.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.57"/>
   </cols>
@@ -1179,4 +1449,543 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:BB5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BA2" activeCellId="0" sqref="BA2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AO1" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AP1" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="AQ1" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS1" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="AT1" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="AU1" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AW1" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AX1" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AY1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA1" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AP2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AQ2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AR2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AT2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AU2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AX2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AY2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="AZ2" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="BA2" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="U3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="AD5" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE5" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AF5" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG5" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH5" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI5" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ5" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK5" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL5" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AM5" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN5" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO5" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP5" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="AQ5" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AR5" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="AS5" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="AT5" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AU5" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AV5" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="AW5" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="AX5" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="AY5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="AZ5" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="BA5" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="BB5" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated ActionHelper, JavaScriptHelper, CommonMethod, BaseClass with NGWebDriver and Building Test Cases
</commit_message>
<xml_diff>
--- a/TestData/RegressionTestData.xlsx
+++ b/TestData/RegressionTestData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="210">
   <si>
     <t xml:space="preserve">CityProjectName</t>
   </si>
@@ -220,6 +220,18 @@
     <t xml:space="preserve">HealthSafetyVoilentCrime _Remarks</t>
   </si>
   <si>
+    <t xml:space="preserve">ManagingEntityName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ManagingEntityAdd1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ManagingEntityAdd2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ManagingEntityCity</t>
+  </si>
+  <si>
     <t xml:space="preserve">Init@pass1</t>
   </si>
   <si>
@@ -284,6 +296,18 @@
   </si>
   <si>
     <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Managing Entity Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Managing Entity Address1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Managing Entity Address 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Managing Entity City</t>
   </si>
   <si>
     <t xml:space="preserve">MS_OperatingHours_Hour</t>
@@ -443,14 +467,15 @@
         <color rgb="FF3F7F5F"/>
         <rFont val="Consolas"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Dichlorobenzene</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <rFont val=""/>
-        <family val="1"/>
+        <rFont val="Consolas"/>
+        <family val="0"/>
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">_Reading</t>
@@ -460,6 +485,87 @@
     <t xml:space="preserve">Formaldehyde_Reading</t>
   </si>
   <si>
+    <t xml:space="preserve">FMS_Q1_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q1_Contact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q2_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q3_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q5_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q6_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q7_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q8_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q9_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q10_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q11_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q12_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q13_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q14_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q15_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q16_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q17_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q18_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FMS_Q19_Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q3_WhomToContact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q4_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q5_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q6_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q7_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q8_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q9_Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_Q10_Location</t>
+  </si>
+  <si>
     <t xml:space="preserve">3 Hours</t>
   </si>
   <si>
@@ -536,6 +642,36 @@
   </si>
   <si>
     <t xml:space="preserve">Regular Occupant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.linkedin.com/company/promantus-inc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M- 0124-34563, Gurgaon,HR, India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Administer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disease control Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupant screening Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hand washing and disinfection Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facility support social distancing Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintain social distance Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">protected from disease transmission Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">facilities staff use PPE appropriately Location</t>
   </si>
 </sst>
 </file>
@@ -588,11 +724,12 @@
       <color rgb="FF3F7F5F"/>
       <name val="Consolas"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
-      <name val=""/>
-      <family val="1"/>
+      <name val="Consolas"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -739,16 +876,20 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="1" sqref="BA2 N2"/>
+      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="14" style="0" width="11.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,7 +992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I3" s="0" t="n">
         <v>8</v>
       </c>
@@ -884,13 +1025,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="BA2 E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ3" activeCellId="0" sqref="AJ3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
@@ -904,7 +1045,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>31</v>
       </c>
@@ -1007,147 +1148,285 @@
       <c r="AH1" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AI1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>48</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="V2" s="0" t="s">
         <v>52</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>54</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AI2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>94</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="I3" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>9</v>
+      </c>
       <c r="K3" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="L3" s="0" t="n">
+        <v>11</v>
+      </c>
       <c r="M3" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="N3" s="0" t="n">
+        <v>13</v>
+      </c>
       <c r="O3" s="0" t="n">
         <v>14</v>
       </c>
+      <c r="P3" s="0" t="n">
+        <v>15</v>
+      </c>
       <c r="Q3" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="R3" s="0" t="n">
+        <v>17</v>
+      </c>
       <c r="S3" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="T3" s="0" t="n">
+        <v>19</v>
+      </c>
       <c r="U3" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="V3" s="0" t="n">
+        <v>21</v>
+      </c>
       <c r="W3" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="X3" s="0" t="n">
+        <v>23</v>
+      </c>
       <c r="Y3" s="0" t="n">
         <v>24</v>
       </c>
+      <c r="Z3" s="0" t="n">
+        <v>25</v>
+      </c>
       <c r="AA3" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="AB3" s="0" t="n">
+        <v>27</v>
+      </c>
       <c r="AC3" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="AD3" s="0" t="n">
+        <v>29</v>
+      </c>
       <c r="AE3" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="AR3" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="AS3" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="AT3" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AU3" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AV3" s="0" t="n">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1173,10 +1452,10 @@
   <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="BA2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
@@ -1190,7 +1469,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1016" style="0" width="11.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>31</v>
       </c>
@@ -1294,111 +1573,111 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>48</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="V2" s="0" t="s">
         <v>52</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>54</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I3" s="0" t="n">
         <v>8</v>
       </c>
@@ -1456,337 +1735,501 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BB5"/>
+  <dimension ref="A1:DJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BA2" activeCellId="0" sqref="BA2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BU1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CB2" activeCellId="0" sqref="CB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="4" style="0" width="11.76"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
+      </c>
+      <c r="BB1" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="BC1" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="BD1" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="BE1" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="BF1" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="BG1" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="BH1" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="BI1" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="BJ1" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="BK1" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="BL1" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="BM1" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="BN1" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="BO1" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="BP1" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="BQ1" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR1" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="BS1" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="BT1" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="BU1" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="BV1" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="BW1" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="BX1" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="BY1" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="BZ1" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="CA1" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="CB1" s="0" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>141</v>
+        <v>176</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>144</v>
+        <v>179</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>143</v>
+        <v>178</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>142</v>
+        <v>177</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>164</v>
+        <v>199</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AT2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AV2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AW2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AX2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="BA2" s="0" t="s">
-        <v>155</v>
+        <v>190</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BC2" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="BD2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BE2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BF2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BG2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BH2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BI2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BJ2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BK2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BL2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BM2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BN2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BO2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BP2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BQ2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BR2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BS2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BT2" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="BU2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="BV2" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="BW2" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="BX2" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="BY2" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="BZ2" s="0" t="s">
+        <v>207</v>
+      </c>
+      <c r="CA2" s="0" t="s">
+        <v>208</v>
+      </c>
+      <c r="CB2" s="0" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,8 +2421,208 @@
       <c r="BB5" s="0" t="n">
         <v>53</v>
       </c>
+      <c r="BC5" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="BD5" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="BE5" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="BF5" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="BG5" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="BH5" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="BI5" s="0" t="n">
+        <v>60</v>
+      </c>
+      <c r="BJ5" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="BK5" s="0" t="n">
+        <v>62</v>
+      </c>
+      <c r="BL5" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="BM5" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="BN5" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="BO5" s="0" t="n">
+        <v>66</v>
+      </c>
+      <c r="BP5" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="BQ5" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="BR5" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="BS5" s="0" t="n">
+        <v>70</v>
+      </c>
+      <c r="BT5" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="BU5" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="BV5" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="BW5" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="BX5" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="BY5" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="BZ5" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="CA5" s="0" t="n">
+        <v>78</v>
+      </c>
+      <c r="CB5" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="CC5" s="0" t="n">
+        <v>80</v>
+      </c>
+      <c r="CD5" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="CE5" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="CF5" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="CG5" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="CH5" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="CI5" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="CJ5" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="CK5" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="CL5" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="CM5" s="0" t="n">
+        <v>90</v>
+      </c>
+      <c r="CN5" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="CO5" s="0" t="n">
+        <v>92</v>
+      </c>
+      <c r="CP5" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="CQ5" s="0" t="n">
+        <v>94</v>
+      </c>
+      <c r="CR5" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="CS5" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="CT5" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="CU5" s="0" t="n">
+        <v>98</v>
+      </c>
+      <c r="CV5" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="CW5" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="CX5" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="CY5" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="CZ5" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="DA5" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="DB5" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="DC5" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="DD5" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="DE5" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="DF5" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="DG5" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="DH5" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="DI5" s="0" t="n">
+        <v>112</v>
+      </c>
+      <c r="DJ5" s="0" t="n">
+        <v>113</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="BB2" r:id="rId1" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BD2" r:id="rId2" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BE2" r:id="rId3" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BF2" r:id="rId4" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BG2" r:id="rId5" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BH2" r:id="rId6" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BI2" r:id="rId7" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BJ2" r:id="rId8" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BK2" r:id="rId9" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BL2" r:id="rId10" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BM2" r:id="rId11" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BN2" r:id="rId12" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BO2" r:id="rId13" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BP2" r:id="rId14" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BQ2" r:id="rId15" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BR2" r:id="rId16" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BS2" r:id="rId17" display="https://www.linkedin.com/company/promantus-inc"/>
+    <hyperlink ref="BT2" r:id="rId18" display="https://www.linkedin.com/company/promantus-inc"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Updating Test Data file
</commit_message>
<xml_diff>
--- a/TestData/RegressionTestData.xlsx
+++ b/TestData/RegressionTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectRegistration" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="216">
   <si>
     <t xml:space="preserve">CityProjectName</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">BuildingOwnerCountry</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCity</t>
+    <t xml:space="preserve">AutoCity-</t>
   </si>
   <si>
     <t xml:space="preserve">1130</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">20037</t>
   </si>
   <si>
-    <t xml:space="preserve">TestCommunities</t>
+    <t xml:space="preserve">AutoCommunity-</t>
   </si>
   <si>
     <t xml:space="preserve">Auto-Building-</t>
@@ -232,6 +232,15 @@
     <t xml:space="preserve">ManagingEntityCity</t>
   </si>
   <si>
+    <t xml:space="preserve">ManagingEntityState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USGBC_UnregisteredUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ScoreVersion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Init@pass1</t>
   </si>
   <si>
@@ -308,6 +317,15 @@
   </si>
   <si>
     <t xml:space="preserve">Test Managing Entity City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">narayanarc211@gmail.com </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.0</t>
   </si>
   <si>
     <t xml:space="preserve">MS_OperatingHours_Hour</t>
@@ -875,11 +893,11 @@
   </sheetPr>
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AO1:AO2 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
@@ -1027,8 +1045,8 @@
   </sheetPr>
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ3" activeCellId="0" sqref="AJ3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1:AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1161,10 +1179,13 @@
         <v>68</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="AO1" s="0" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1172,115 +1193,124 @@
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>48</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="V2" s="0" t="s">
         <v>52</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>54</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>64</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,10 +1479,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1:AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1572,109 +1602,151 @@
       <c r="AH1" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="AI1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO1" s="0" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="R2" s="0" t="s">
         <v>48</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="T2" s="0" t="s">
         <v>50</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="V2" s="0" t="s">
         <v>52</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>54</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>56</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>58</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>60</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>62</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>64</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AO2" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,8 +1783,47 @@
       <c r="AC3" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="AD3" s="0" t="n">
+        <v>29</v>
+      </c>
       <c r="AE3" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="AF3" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="AH3" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI3" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AJ3" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="AK3" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="AL3" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AM3" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="AN3" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="AO3" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AP3" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="AQ3" s="0" t="n">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1737,11 +1848,11 @@
   </sheetPr>
   <dimension ref="A1:DJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BU1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CB2" activeCellId="0" sqref="CB2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BU1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="CB2" activeCellId="1" sqref="AO1:AO2 CB2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
@@ -1750,486 +1861,486 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="BT1" s="0" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="BU1" s="0" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="BV1" s="0" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="BW1" s="0" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="BX1" s="0" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="BY1" s="0" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="BZ1" s="0" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="CA1" s="0" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="CB1" s="0" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="K2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="P2" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="Q2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE2" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="M2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>185</v>
-      </c>
-      <c r="O2" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="P2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>187</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>189</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>190</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>191</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>194</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>178</v>
-      </c>
       <c r="AG2" s="0" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="AK2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="AM2" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="AN2" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="AO2" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="AL2" s="0" t="s">
-        <v>197</v>
-      </c>
-      <c r="AM2" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>199</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>190</v>
-      </c>
       <c r="AP2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AT2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AV2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AW2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AX2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="BA2" s="0" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BC2" s="0" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BG2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BP2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BT2" s="2" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="BU2" s="0" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="BV2" s="0" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="BW2" s="0" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="BX2" s="0" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="BY2" s="0" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="BZ2" s="0" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="CA2" s="0" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="CB2" s="0" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Adding changes related to parksmart
</commit_message>
<xml_diff>
--- a/TestData/RegressionTestData.xlsx
+++ b/TestData/RegressionTestData.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectRegistration" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="City" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Communities" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Building" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Parking" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="241">
   <si>
     <t xml:space="preserve">CityProjectName</t>
   </si>
@@ -73,6 +74,42 @@
     <t xml:space="preserve">BuildingOwnerCountry</t>
   </si>
   <si>
+    <t xml:space="preserve">ParkingProjectName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingGrossArea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingSpace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingLevel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingOwnerType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingOwnerOrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingOwnerEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ParkingOwnerCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BillingName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CVV</t>
+  </si>
+  <si>
     <t xml:space="preserve">AutoCity-</t>
   </si>
   <si>
@@ -118,6 +155,36 @@
     <t xml:space="preserve">narayanarc21@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">TestParking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP ARCHITECTURE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apandey6555@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4111111111111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999</t>
+  </si>
+  <si>
     <t xml:space="preserve">UpdatedByEmailId</t>
   </si>
   <si>
@@ -266,9 +333,6 @@
   </si>
   <si>
     <t xml:space="preserve">Water Consumption Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
   </si>
   <si>
     <t xml:space="preserve">Waste Generation Remarks</t>
@@ -690,6 +754,18 @@
   </si>
   <si>
     <t xml:space="preserve">facilities staff use PPE appropriately Location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usgbc_Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arc_Admin_Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TeamMemberEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbisht@usgbc.org</t>
   </si>
 </sst>
 </file>
@@ -891,13 +967,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AO1:AO2 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
@@ -907,7 +983,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="14" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="14" style="0" width="11.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,55 +1035,127 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1018,15 +1166,25 @@
         <v>10</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P3" s="0" t="n">
         <v>14</v>
+      </c>
+      <c r="Q3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="V3" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="AB3" s="0" t="n">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" display="narayanarc21@gmail.com"/>
+    <hyperlink ref="W2" r:id="rId2" display="apandey6555@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1046,7 +1204,7 @@
   <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1:AO2"/>
+      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1065,252 +1223,252 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="U2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="W2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="AA2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="AC2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="AE2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" s="0" t="s">
+      <c r="AG2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AI2" s="0" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1481,8 +1639,8 @@
   </sheetPr>
   <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1:AO2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1501,252 +1659,252 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="T2" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="U2" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="V2" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F2" s="0" t="s">
+      <c r="W2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="X2" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="Y2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z2" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="0" t="s">
+      <c r="AA2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="L2" s="0" t="s">
+      <c r="AC2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="N2" s="0" t="s">
+      <c r="AE2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="O2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" s="0" t="s">
+      <c r="AG2" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AI2" s="0" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>97</v>
+        <v>118</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1849,10 +2007,10 @@
   <dimension ref="A1:DJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BU1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CB2" activeCellId="1" sqref="AO1:AO2 CB2"/>
+      <selection pane="topLeft" activeCell="CD2" activeCellId="0" sqref="CD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
@@ -1861,486 +2019,486 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>104</v>
+        <v>125</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>118</v>
+        <v>139</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>119</v>
+        <v>140</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>120</v>
+        <v>141</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>121</v>
+        <v>142</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>123</v>
+        <v>144</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>137</v>
+        <v>158</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
       <c r="AY1" s="4" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="AZ1" s="4" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="BB1" s="0" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="BC1" s="0" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="BD1" s="0" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="BE1" s="0" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="BF1" s="0" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="BG1" s="0" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="BH1" s="0" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="BI1" s="0" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="BJ1" s="0" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="BK1" s="0" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="BL1" s="0" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="BM1" s="0" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="BN1" s="0" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="BO1" s="0" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="BP1" s="0" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="BQ1" s="0" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="BR1" s="0" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="BS1" s="0" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="BT1" s="0" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="BU1" s="0" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="BV1" s="0" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="BW1" s="0" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="BX1" s="0" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="BY1" s="0" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="BZ1" s="0" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="CA1" s="0" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="CB1" s="0" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>187</v>
+        <v>208</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>191</v>
+        <v>212</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>192</v>
+        <v>213</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>195</v>
+        <v>216</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>85</v>
+        <v>106</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>199</v>
+        <v>220</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>200</v>
+        <v>221</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>201</v>
+        <v>222</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>202</v>
+        <v>223</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>203</v>
+        <v>224</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>204</v>
+        <v>225</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>205</v>
+        <v>226</v>
       </c>
       <c r="AO2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AT2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AU2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AV2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AW2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AX2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="AZ2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="BA2" s="0" t="s">
-        <v>196</v>
+        <v>217</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BC2" s="0" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BG2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BI2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BJ2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BK2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BL2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BM2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BN2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BO2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BP2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BQ2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BR2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BS2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BT2" s="2" t="s">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="BU2" s="0" t="s">
-        <v>208</v>
+        <v>229</v>
       </c>
       <c r="BV2" s="0" t="s">
-        <v>209</v>
+        <v>230</v>
       </c>
       <c r="BW2" s="0" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="BX2" s="0" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="BY2" s="0" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="BZ2" s="0" t="s">
-        <v>213</v>
+        <v>234</v>
       </c>
       <c r="CA2" s="0" t="s">
-        <v>214</v>
+        <v>235</v>
       </c>
       <c r="CB2" s="0" t="s">
-        <v>215</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2742,4 +2900,55 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="tbisht@usgbc.org"/>
+    <hyperlink ref="B2" r:id="rId2" display="narayanarc21@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId3" display="apandey6555@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Transit Project Registration Module
</commit_message>
<xml_diff>
--- a/TestData/RegressionTestData.xlsx
+++ b/TestData/RegressionTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectRegistration" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Communities" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Building" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Parking" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="TransitRegistration" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="269">
   <si>
     <t xml:space="preserve">CityProjectName</t>
   </si>
@@ -756,16 +757,100 @@
     <t xml:space="preserve">facilities staff use PPE appropriately Location</t>
   </si>
   <si>
-    <t xml:space="preserve">Registered_User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unregistered_User </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternate_User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apandey9698@icloud.com</t>
+    <t xml:space="preserve">Usgbc_Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arc_Admin_Username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TeamMemberEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbisht@usgbc.org</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initpass@21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_Name_UG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_Name_AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annual_Rider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weekly_Hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fulltime_Staff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg_time_Spent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross_Area </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TransitAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit_Zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpaceType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OwnerType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">OwnerOrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OwnerEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OwnerRegion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Card_Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutoTransit-UG-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutoTransit-AG-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123456</t>
+  </si>
+  <si>
+    <t xml:space="preserve">102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40087</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transit: Station</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test User </t>
   </si>
 </sst>
 </file>
@@ -775,7 +860,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -826,6 +911,11 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -869,7 +959,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -887,6 +977,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -969,11 +1063,11 @@
   </sheetPr>
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="S1:U2 D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
@@ -983,7 +1077,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="14" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="14" style="0" width="11.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="31" style="0" width="11.84"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,7 +1301,7 @@
   <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1"/>
+      <selection pane="topLeft" activeCell="AO1" activeCellId="1" sqref="S1:U2 AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1640,7 +1737,7 @@
   <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="AO1" activeCellId="1" sqref="S1:U2 AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2006,11 +2103,11 @@
   </sheetPr>
   <dimension ref="A1:DJ5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BU1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="CD2" activeCellId="0" sqref="CD2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S1:U2 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
   </cols>
@@ -2905,51 +3002,282 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="S1:U2 D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="tbisht@usgbc.org"/>
+    <hyperlink ref="B2" r:id="rId2" display="narayanarc21@gmail.com"/>
+    <hyperlink ref="C2" r:id="rId3" display="apandey6555@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId4" display="Initpass@21"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1:U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>237</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>238</v>
+        <v>242</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>54</v>
+        <v>245</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>94</v>
+      <c r="Q2" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="3"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="N4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="R4" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="U4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="V4" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="W4" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="X4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y4" s="0" t="n">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="apandey6555@gmail.com"/>
-    <hyperlink ref="B2" r:id="rId2" display="apandey9698@icloud.com"/>
-    <hyperlink ref="C2" r:id="rId3" display="narayanarc21@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId4" display="Init@pass1"/>
+    <hyperlink ref="P2" r:id="rId1" display="apandey6555@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fix for Parking teams testcases
</commit_message>
<xml_diff>
--- a/TestData/RegressionTestData.xlsx
+++ b/TestData/RegressionTestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectRegistration" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="268">
   <si>
     <t xml:space="preserve">CityProjectName</t>
   </si>
@@ -757,19 +757,16 @@
     <t xml:space="preserve">facilities staff use PPE appropriately Location</t>
   </si>
   <si>
-    <t xml:space="preserve">Usgbc_Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arc_Admin_Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TeamMemberEmail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tbisht@usgbc.org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Initpass@21</t>
+    <t xml:space="preserve">UnRegistered User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ExistingMember</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registered User</t>
+  </si>
+  <si>
+    <t xml:space="preserve">apandey09@icloud.com</t>
   </si>
   <si>
     <t xml:space="preserve">Transit_Name_UG</t>
@@ -912,9 +909,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1064,10 +1063,10 @@
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="S1:U2 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.94"/>
@@ -1301,7 +1300,7 @@
   <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO1" activeCellId="1" sqref="S1:U2 AO1"/>
+      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1737,7 +1736,7 @@
   <dimension ref="A1:AQ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO1" activeCellId="1" sqref="S1:U2 AO1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2104,10 +2103,10 @@
   <dimension ref="A1:DJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="S1:U2 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.04"/>
   </cols>
@@ -3004,11 +3003,11 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="S1:U2 D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3034,16 +3033,16 @@
       <c r="C2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>241</v>
+      <c r="D2" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="tbisht@usgbc.org"/>
+    <hyperlink ref="A2" r:id="rId1" display="apandey09@icloud"/>
     <hyperlink ref="B2" r:id="rId2" display="narayanarc21@gmail.com"/>
     <hyperlink ref="C2" r:id="rId3" display="apandey6555@gmail.com"/>
-    <hyperlink ref="D2" r:id="rId4" display="Initpass@21"/>
+    <hyperlink ref="D2" r:id="rId4" display="Init@pass1"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3062,69 +3061,69 @@
   </sheetPr>
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1:U2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S1" activeCellId="0" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="K1" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="L1" s="0" t="s">
         <v>252</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="M1" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="N1" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="O1" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="P1" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="Q1" s="0" t="s">
         <v>257</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>258</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>24</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="T1" s="0" t="s">
         <v>26</v>
@@ -3135,25 +3134,25 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="0" t="s">
         <v>261</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>262</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>113</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>264</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>265</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>31</v>
@@ -3171,7 +3170,7 @@
         <v>35</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N2" s="0" t="s">
         <v>40</v>
@@ -3183,10 +3182,10 @@
         <v>48</v>
       </c>
       <c r="Q2" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="R2" s="0" t="s">
         <v>267</v>
-      </c>
-      <c r="R2" s="0" t="s">
-        <v>268</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>50</v>

</xml_diff>